<commit_message>
Added row 11, more mermaids
</commit_message>
<xml_diff>
--- a/test book 1.xlsx
+++ b/test book 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github Repositories\Stranding-data_HI-data_SEFSC_SERO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D6C7F9-54E7-498B-BA74-6E1CA45550F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81FCCEA-28A8-47B1-B5EC-1E78C467EDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>Species</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>test 3</t>
+  </si>
+  <si>
+    <t>SER25-00777</t>
+  </si>
+  <si>
+    <t>test 4</t>
   </si>
 </sst>
 </file>
@@ -481,13 +487,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="24" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.08984375" style="3" customWidth="1"/>
@@ -497,7 +503,7 @@
     <col min="6" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -517,7 +523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -534,7 +540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -551,7 +557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -568,7 +574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -585,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -602,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -619,7 +625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -639,7 +645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -659,7 +665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -677,6 +683,26 @@
       </c>
       <c r="F10" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3">
+        <v>60</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>